<commit_message>
Update OSHA Coronavirus-Related Inspections with Violations from August, 2020 - December, 2021.xlsx
cleaning the excel file
</commit_message>
<xml_diff>
--- a/OSHA Coronavirus-Related Inspections with Violations from August, 2020 - December, 2021.xlsx
+++ b/OSHA Coronavirus-Related Inspections with Violations from August, 2020 - December, 2021.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AYOTUNDE DOHERTY\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AYOTUNDE DOHERTY\Documents\OSHA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC62E45C-0974-4C46-8B18-8D98E8EF0C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938935D2-E598-4846-B6FE-45A6C9A596F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{B049947C-0D25-49E2-BE20-A5B32AE9EF29}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2972" uniqueCount="1513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2971" uniqueCount="1512">
   <si>
     <t>Establishment Name</t>
   </si>
@@ -4580,9 +4580,6 @@
   </si>
   <si>
     <t>AKRON</t>
-  </si>
-  <si>
-    <t>, with Total Initial Penalties of $4,034,288</t>
   </si>
 </sst>
 </file>
@@ -4939,9 +4936,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B124D8E9-3888-499B-A79D-C83C5F66BE66}">
-  <dimension ref="A1:G743"/>
+  <dimension ref="A2:G743"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4954,11 +4953,6 @@
     <col min="7" max="7" width="81.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1512</v>
-      </c>
-    </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Average initial penalty recorded yearly, monthly and quarterly basis
Average initial penalty recorded yearly, monthly and quarterly basis
</commit_message>
<xml_diff>
--- a/OSHA Coronavirus-Related Inspections with Violations from August, 2020 - December, 2021.xlsx
+++ b/OSHA Coronavirus-Related Inspections with Violations from August, 2020 - December, 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AYOTUNDE DOHERTY\Documents\OSHA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938935D2-E598-4846-B6FE-45A6C9A596F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F926EA1-7FF3-4E25-B4AB-169B9048F24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{B049947C-0D25-49E2-BE20-A5B32AE9EF29}"/>
   </bookViews>
@@ -4586,13 +4586,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -4615,9 +4621,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4936,10 +4943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B124D8E9-3888-499B-A79D-C83C5F66BE66}">
-  <dimension ref="A2:G743"/>
+  <dimension ref="A1:G743"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4953,6 +4960,9 @@
     <col min="7" max="7" width="81.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C1" s="2"/>
+    </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>

</xml_diff>